<commit_message>
20 digit for chewy is working. Need to think of a better way to streamline?
</commit_message>
<xml_diff>
--- a/assets/Chewy/Chewy 856 ASN - Copy.xlsx
+++ b/assets/Chewy/Chewy 856 ASN - Copy.xlsx
@@ -177,7 +177,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,32 +188,25 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -370,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -405,25 +398,16 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
@@ -435,6 +419,9 @@
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -459,7 +446,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -785,24 +772,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="33" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="34" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="35" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="33" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="36" width="18.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="37" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="33" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="33" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="33" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="33" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="33" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="33" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="31" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="32" width="19.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="33" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="31" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="34" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="35" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="31" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="31" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="31" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="31" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="31" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="31" width="20.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -979,10 +966,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2"/>
-      <c r="B10" s="12"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="12"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
@@ -992,12 +979,18 @@
       <c r="L10" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="5"/>
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="B11" s="12"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="5"/>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -1007,16 +1000,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="B12" s="13"/>
       <c r="C12" s="2"/>
       <c r="D12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="F12" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="5"/>
@@ -1025,22 +1020,22 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="15"/>
       <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E13" s="8"/>
       <c r="F13" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -1049,18 +1044,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="18"/>
+        <v>33</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E14" s="8"/>
       <c r="F14" s="6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -1071,17 +1064,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="16"/>
+        <v>35</v>
+      </c>
+      <c r="B15" s="13"/>
       <c r="C15" s="2"/>
       <c r="D15" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E15" s="8"/>
-      <c r="F15" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1091,14 +1082,12 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="8"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="2"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1108,13 +1097,11 @@
       <c r="L16" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="12"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1124,116 +1111,102 @@
       <c r="L17" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="2"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="D18" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="21"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="23"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="23"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
+      <c r="A19" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="D19" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
+        <v>43</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>47</v>
+      </c>
       <c r="I19" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J19" s="25"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="25"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="I20" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="26" t="s">
+      <c r="J19" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="K20" s="26" t="s">
+      <c r="K19" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="L20" s="26" t="s">
+      <c r="L19" s="24" t="s">
         <v>51</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="27"/>
+    </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="29"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="29"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="29"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="27"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>